<commit_message>
Small tweaks to URIs
 - URIs for narrower items are not hierarchical (because they could
   have more than one broader term, in theory)
 - identifiers use underscore instead of hyphen (we're not yet
   consistent about this unfortunately elsewhere.)
</commit_message>
<xml_diff>
--- a/excel2skos-holocaust_geographies2.xlsx
+++ b/excel2skos-holocaust_geographies2.xlsx
@@ -27,7 +27,7 @@
     <t xml:space="preserve">ConceptScheme URI</t>
   </si>
   <si>
-    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri-holocaust-geographies</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies</t>
   </si>
   <si>
     <t xml:space="preserve">dct:title@en</t>
@@ -60,79 +60,79 @@
     <t xml:space="preserve">skos:notation</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/places-of-persecution</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/places_of_persecution</t>
   </si>
   <si>
     <t xml:space="preserve">Places of persecution</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/places-of-persecution/ghettos</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/ghettos</t>
   </si>
   <si>
     <t xml:space="preserve">Ghettos</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/places-of-persecution/camps</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/camps</t>
   </si>
   <si>
     <t xml:space="preserve">Concentration camps</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/places-of-persecution/other_extermination</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/other_extermination</t>
   </si>
   <si>
     <t xml:space="preserve">Other sites of extermination</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/places-of-persecution/sites_violence</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/sites_violence</t>
   </si>
   <si>
     <t xml:space="preserve">Sites of violence</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/places-of-persecution/forced_labour</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/forced_labour</t>
   </si>
   <si>
     <t xml:space="preserve">Places of forced labour</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/borders</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/borders</t>
   </si>
   <si>
     <t xml:space="preserve">Borders</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/borders/state</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/borders/state</t>
   </si>
   <si>
     <t xml:space="preserve">State borders</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/borders/administrative</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/borders/administrative</t>
   </si>
   <si>
     <t xml:space="preserve">Administrative borders</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/local</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/local</t>
   </si>
   <si>
     <t xml:space="preserve">Local history</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/local/community</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/community</t>
   </si>
   <si>
     <t xml:space="preserve">Communities</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/local/residence</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/residence</t>
   </si>
   <si>
     <t xml:space="preserve">Places of residence</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/local/religious</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/religious</t>
   </si>
   <si>
     <t xml:space="preserve">Religious life</t>
@@ -141,7 +141,7 @@
     <t xml:space="preserve">Typically places and objects like synagogues, cemeteries, etc.</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/local/memorial</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/memorial</t>
   </si>
   <si>
     <t xml:space="preserve">Memorial places</t>
@@ -150,13 +150,13 @@
     <t xml:space="preserve">Memorials, museums, memorial plagues, Stolpersteine, etc.</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/local/hiding</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/hiding</t>
   </si>
   <si>
     <t xml:space="preserve">Hiding places</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/local/incidents</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/incidents</t>
   </si>
   <si>
     <t xml:space="preserve">Incidents</t>
@@ -165,7 +165,7 @@
     <t xml:space="preserve">Typically microhistorical interactions which include incidents like arrests, denunciations, controls, etc.</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/forced_mobility</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/forced_mobility</t>
   </si>
   <si>
     <t xml:space="preserve">Forced mobility</t>
@@ -174,61 +174,61 @@
     <t xml:space="preserve">As of now, mixes infrastructure and movement of people. To be re-conceptualised…</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/forced_mobility/assembly_points</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/assembly_points</t>
   </si>
   <si>
     <t xml:space="preserve">Assembly points</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/forced_mobility/transport_lines</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/transport_lines</t>
   </si>
   <si>
     <t xml:space="preserve">Railways and transport lines</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/forced_mobility/deportations</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/deportations</t>
   </si>
   <si>
     <t xml:space="preserve">Deportations</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/forced_mobility/death_marches</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/death_marches</t>
   </si>
   <si>
     <t xml:space="preserve">Death marches</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/refugee_spaces</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/refugee_spaces</t>
   </si>
   <si>
     <t xml:space="preserve">Refugee spaces</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/refugee_spaces/refugee_camps</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/refugee_camps</t>
   </si>
   <si>
     <t xml:space="preserve">Refugee camps</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/refugee_spaces/border_crossings</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/border_crossings</t>
   </si>
   <si>
     <t xml:space="preserve">Border crossings</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/refugee_spaces/boat_passages</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/boat_passages</t>
   </si>
   <si>
     <t xml:space="preserve">Boat passages</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/refugee_spaces/consulates</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/consulates</t>
   </si>
   <si>
     <t xml:space="preserve">Consulates</t>
   </si>
   <si>
-    <t xml:space="preserve">https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/refugee_spaces/aid_organisations</t>
+    <t xml:space="preserve">http://data.ehri-project.eu/vocabularies/ehri_holocaust_geographies/aid_organisations</t>
   </si>
   <si>
     <t xml:space="preserve">Aid organisations</t>
@@ -426,14 +426,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A34 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -449,12 +449,12 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="112.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="45.71"/>
@@ -621,7 +621,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>32</v>
       </c>
@@ -816,41 +816,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="title@en"/>
-    <hyperlink ref="A3" r:id="rId2" display="description@en"/>
-    <hyperlink ref="B7" r:id="rId3" display="prefLabel@en"/>
-    <hyperlink ref="C7" r:id="rId4" display="definition@en"/>
-    <hyperlink ref="A12" r:id="rId5" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/places-of-persecution/sites_violence"/>
-    <hyperlink ref="A13" r:id="rId6" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/places-of-persecution/forced_labour"/>
-    <hyperlink ref="A15" r:id="rId7" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/borders/state"/>
-    <hyperlink ref="A16" r:id="rId8" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/borders/administrative"/>
-    <hyperlink ref="A17" r:id="rId9" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/local"/>
-    <hyperlink ref="A18" r:id="rId10" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/local/community"/>
-    <hyperlink ref="D18" r:id="rId11" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/local"/>
-    <hyperlink ref="D19" r:id="rId12" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/local"/>
-    <hyperlink ref="D20" r:id="rId13" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/local"/>
-    <hyperlink ref="D21" r:id="rId14" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/local"/>
-    <hyperlink ref="D22" r:id="rId15" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/local"/>
-    <hyperlink ref="D23" r:id="rId16" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/local"/>
-    <hyperlink ref="A25" r:id="rId17" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/forced_mobility/assembly_points"/>
-    <hyperlink ref="A26" r:id="rId18" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/forced_mobility/transport_lines"/>
-    <hyperlink ref="A27" r:id="rId19" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/forced_mobility/deportations"/>
-    <hyperlink ref="A28" r:id="rId20" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/forced_mobility/death_marches"/>
-    <hyperlink ref="A29" r:id="rId21" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/refugee_spaces"/>
-    <hyperlink ref="A30" r:id="rId22" display="https://portal.ehri"/>
-    <hyperlink ref="D30" r:id="rId23" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/refugee_spaces"/>
-    <hyperlink ref="A31" r:id="rId24" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/refugee_spaces/border_crossings"/>
-    <hyperlink ref="D31" r:id="rId25" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/refugee_spaces"/>
-    <hyperlink ref="A32" r:id="rId26" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/refugee_spaces/boat_passages"/>
-    <hyperlink ref="D32" r:id="rId27" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/refugee_spaces"/>
-    <hyperlink ref="A33" r:id="rId28" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/refugee_spaces/consulates"/>
-    <hyperlink ref="D33" r:id="rId29" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/refugee_spaces"/>
-    <hyperlink ref="A34" r:id="rId30" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/refugee_spaces/aid_organisations"/>
-    <hyperlink ref="D34" r:id="rId31" display="https://portal.ehri-project.eu/vocabularies/ehri-holocaust-geographies/refugee_spaces"/>
+    <hyperlink ref="A2" r:id="rId1" display="dct:title@en"/>
+    <hyperlink ref="A3" r:id="rId2" display="dct:description@en"/>
+    <hyperlink ref="B7" r:id="rId3" display="skos:prefLabel@en"/>
+    <hyperlink ref="C7" r:id="rId4" display="skos:definition@en"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -866,14 +839,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A34 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>